<commit_message>
Project Example 2 - Corporate Rating is saved. Type: SAVE.
</commit_message>
<xml_diff>
--- a/DESIGN/rules/Example 2 - Corporate Rating/Corporate Rating.xlsx
+++ b/DESIGN/rules/Example 2 - Corporate Rating/Corporate Rating.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="931" uniqueCount="506">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="932" uniqueCount="507">
   <si>
     <t>Domain Model</t>
   </si>
@@ -3503,11 +3503,15 @@
       <t>(Double value)</t>
     </r>
   </si>
+  <si>
+    <t>tests123</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="27" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -3692,7 +3696,7 @@
     </font>
     <font>
       <sz val="10"/>
-      <color theme="0" tint="-0.34998626667073579"/>
+      <color theme="0" tint="-0.34998626667073579" rgb="FFFFFF"/>
       <name val="Franklin Gothic Book"/>
       <family val="2"/>
       <charset val="204"/>
@@ -3729,7 +3733,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
+        <fgColor theme="0" rgb="FFFFFF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3741,13 +3745,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <fgColor theme="0" tint="-0.34998626667073579" rgb="FFFFFF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="2" tint="-0.249977111117893"/>
+        <fgColor theme="2" tint="-0.249977111117893" rgb="FBEEC9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3759,7 +3763,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <fgColor theme="0" tint="-0.14999847407452621" rgb="FFFFFF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3924,9 +3928,9 @@
     </border>
   </borders>
   <cellStyleXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0" xfId="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0" xfId="2"/>
   </cellStyleXfs>
   <cellXfs count="158">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -4313,9 +4317,9 @@
     </xf>
   </cellXfs>
   <cellStyles count="3">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Heading 2" xfId="1" builtinId="17"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -4732,10 +4736,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="12" customWidth="1"/>
-    <col min="4" max="4" width="13" customWidth="1"/>
-    <col min="5" max="5" width="40.90625" customWidth="1"/>
-    <col min="6" max="6" width="56.1796875" customWidth="1"/>
+    <col min="3" max="3" customWidth="true" width="12.0"/>
+    <col min="4" max="4" customWidth="true" width="13.0"/>
+    <col min="5" max="5" customWidth="true" width="40.90625"/>
+    <col min="6" max="6" customWidth="true" width="56.1796875"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:8" ht="22.2" thickBot="1" x14ac:dyDescent="0.5">
@@ -4830,7 +4834,9 @@
         <v>459</v>
       </c>
       <c r="D12" s="123"/>
-      <c r="E12" s="112"/>
+      <c r="E12" s="112" t="s">
+        <v>506</v>
+      </c>
       <c r="F12" s="45" t="s">
         <v>340</v>
       </c>
@@ -6063,8 +6069,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="4" max="4" width="20.81640625" customWidth="1"/>
-    <col min="5" max="5" width="57.90625" customWidth="1"/>
+    <col min="4" max="4" customWidth="true" width="20.81640625"/>
+    <col min="5" max="5" customWidth="true" width="57.90625"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:7" x14ac:dyDescent="0.35">
@@ -6275,9 +6281,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="12.08984375" customWidth="1"/>
-    <col min="3" max="3" width="24.1796875" customWidth="1"/>
-    <col min="4" max="4" width="36.81640625" customWidth="1"/>
+    <col min="2" max="2" customWidth="true" width="12.08984375"/>
+    <col min="3" max="3" customWidth="true" width="24.1796875"/>
+    <col min="4" max="4" customWidth="true" width="36.81640625"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:6" x14ac:dyDescent="0.35">
@@ -6437,11 +6443,11 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="15" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="8.90625" style="1"/>
-    <col min="3" max="3" width="12.6328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="32.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.54296875" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.90625" style="1"/>
+    <col min="1" max="2" style="1" width="8.90625"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="12.6328125"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="32.36328125"/>
+    <col min="5" max="5" customWidth="true" style="1" width="20.54296875"/>
+    <col min="6" max="16384" style="1" width="8.90625"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:6" ht="22.2" thickBot="1" x14ac:dyDescent="0.5">
@@ -7035,9 +7041,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.453125" customWidth="1"/>
-    <col min="2" max="2" width="6" customWidth="1"/>
-    <col min="3" max="3" width="24.08984375" style="19" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="10.453125"/>
+    <col min="2" max="2" customWidth="true" width="6.0"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="19" width="24.08984375"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:4" ht="22.2" thickBot="1" x14ac:dyDescent="0.5">
@@ -7354,11 +7360,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="4" max="4" width="15.08984375" customWidth="1"/>
-    <col min="5" max="5" width="39.36328125" customWidth="1"/>
-    <col min="6" max="6" width="13.6328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.1796875" customWidth="1"/>
-    <col min="9" max="9" width="45.6328125" customWidth="1"/>
+    <col min="4" max="4" customWidth="true" width="15.08984375"/>
+    <col min="5" max="5" customWidth="true" width="39.36328125"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="13.6328125"/>
+    <col min="7" max="7" customWidth="true" width="12.1796875"/>
+    <col min="9" max="9" customWidth="true" width="45.6328125"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:9" ht="22.2" thickBot="1" x14ac:dyDescent="0.5">
@@ -7999,10 +8005,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="11.54296875" customWidth="1"/>
-    <col min="3" max="3" width="21.54296875" customWidth="1"/>
-    <col min="4" max="4" width="34.81640625" customWidth="1"/>
-    <col min="5" max="5" width="23.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" customWidth="true" width="11.54296875"/>
+    <col min="3" max="3" customWidth="true" width="21.54296875"/>
+    <col min="4" max="4" customWidth="true" width="34.81640625"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="23.453125"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:6" ht="22.2" thickBot="1" x14ac:dyDescent="0.5">
@@ -8369,9 +8375,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="23.6328125" style="48" customWidth="1"/>
-    <col min="4" max="4" width="27.453125" style="48" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" customWidth="true" style="48" width="23.6328125"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="48" width="27.453125"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="27.453125"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:7" x14ac:dyDescent="0.35">
@@ -9188,10 +9194,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="25.54296875" customWidth="1"/>
-    <col min="4" max="4" width="22.08984375" customWidth="1"/>
-    <col min="5" max="5" width="25" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" customWidth="true" width="25.54296875"/>
+    <col min="4" max="4" customWidth="true" width="22.08984375"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="25.0"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="22.08984375"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:11" x14ac:dyDescent="0.35">
@@ -9979,9 +9985,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="18.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.81640625" style="77" customWidth="1"/>
-    <col min="5" max="5" width="17.54296875" style="77" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="18.1796875"/>
+    <col min="4" max="4" customWidth="true" style="77" width="21.81640625"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="77" width="17.54296875"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:7" ht="22.2" thickBot="1" x14ac:dyDescent="0.5">
@@ -10223,10 +10229,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="29.54296875" customWidth="1"/>
-    <col min="4" max="4" width="25.6328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.54296875" customWidth="1"/>
-    <col min="8" max="8" width="7.453125" customWidth="1"/>
+    <col min="3" max="3" customWidth="true" width="29.54296875"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="25.6328125"/>
+    <col min="6" max="6" customWidth="true" width="6.54296875"/>
+    <col min="8" max="8" customWidth="true" width="7.453125"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:15" x14ac:dyDescent="0.35">
@@ -11129,8 +11135,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="34.36328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.6328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="34.36328125"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="25.6328125"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:5" ht="22.2" thickBot="1" x14ac:dyDescent="0.5">
@@ -11290,8 +11296,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="39.90625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="39.90625"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="30.08984375"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:6" x14ac:dyDescent="0.35">
@@ -11497,11 +11503,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="12.453125" customWidth="1"/>
-    <col min="4" max="4" width="16.1796875" customWidth="1"/>
-    <col min="5" max="5" width="18" customWidth="1"/>
-    <col min="6" max="6" width="17.08984375" customWidth="1"/>
-    <col min="7" max="7" width="10.6328125" customWidth="1"/>
+    <col min="3" max="3" customWidth="true" width="12.453125"/>
+    <col min="4" max="4" customWidth="true" width="16.1796875"/>
+    <col min="5" max="5" customWidth="true" width="18.0"/>
+    <col min="6" max="6" customWidth="true" width="17.08984375"/>
+    <col min="7" max="7" customWidth="true" width="10.6328125"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:9" x14ac:dyDescent="0.35">

</xml_diff>